<commit_message>
New command to calculate conceptions by age by year
</commit_message>
<xml_diff>
--- a/Conception rates by age and country.xlsx
+++ b/Conception rates by age and country.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/a_baxter_1_research_gla_ac_uk/Documents/R Studio - home folder/teen-preg-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2286432B\OneDrive - University of Glasgow\R Studio - home folder\teen-preg-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Under 16" sheetId="1" r:id="rId1"/>
@@ -454,24 +454,102 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -490,86 +568,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2367,7 +2367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2839,7 +2839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3474,7 +3474,7 @@
   <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AE5" sqref="AE5"/>
@@ -4335,544 +4335,544 @@
       <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="59">
+      <c r="B1" s="85">
         <v>2015</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="58">
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="84">
         <v>2014</v>
       </c>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="59">
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="85">
         <v>2013</v>
       </c>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="58">
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="85"/>
+      <c r="V1" s="85"/>
+      <c r="W1" s="85"/>
+      <c r="X1" s="85"/>
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="84">
         <v>2012</v>
       </c>
-      <c r="AA1" s="59"/>
-      <c r="AB1" s="59"/>
-      <c r="AC1" s="59"/>
-      <c r="AD1" s="59"/>
-      <c r="AE1" s="59"/>
-      <c r="AF1" s="59"/>
-      <c r="AG1" s="60"/>
-      <c r="AH1" s="70">
+      <c r="AA1" s="85"/>
+      <c r="AB1" s="85"/>
+      <c r="AC1" s="85"/>
+      <c r="AD1" s="85"/>
+      <c r="AE1" s="85"/>
+      <c r="AF1" s="85"/>
+      <c r="AG1" s="86"/>
+      <c r="AH1" s="81">
         <v>2011</v>
       </c>
-      <c r="AI1" s="71"/>
-      <c r="AJ1" s="71"/>
-      <c r="AK1" s="71"/>
-      <c r="AL1" s="71"/>
-      <c r="AM1" s="71"/>
-      <c r="AN1" s="72"/>
+      <c r="AI1" s="82"/>
+      <c r="AJ1" s="82"/>
+      <c r="AK1" s="82"/>
+      <c r="AL1" s="82"/>
+      <c r="AM1" s="82"/>
+      <c r="AN1" s="83"/>
       <c r="AO1" s="27"/>
-      <c r="AP1" s="70">
+      <c r="AP1" s="81">
         <v>2010</v>
       </c>
-      <c r="AQ1" s="71"/>
-      <c r="AR1" s="71"/>
-      <c r="AS1" s="71"/>
-      <c r="AT1" s="71"/>
-      <c r="AU1" s="71"/>
-      <c r="AV1" s="72"/>
+      <c r="AQ1" s="82"/>
+      <c r="AR1" s="82"/>
+      <c r="AS1" s="82"/>
+      <c r="AT1" s="82"/>
+      <c r="AU1" s="82"/>
+      <c r="AV1" s="83"/>
       <c r="AW1" s="27"/>
-      <c r="AX1" s="58">
+      <c r="AX1" s="84">
         <v>2009</v>
       </c>
-      <c r="AY1" s="59"/>
-      <c r="AZ1" s="59"/>
-      <c r="BA1" s="59"/>
-      <c r="BB1" s="59"/>
-      <c r="BC1" s="59"/>
-      <c r="BD1" s="59"/>
-      <c r="BE1" s="60"/>
+      <c r="AY1" s="85"/>
+      <c r="AZ1" s="85"/>
+      <c r="BA1" s="85"/>
+      <c r="BB1" s="85"/>
+      <c r="BC1" s="85"/>
+      <c r="BD1" s="85"/>
+      <c r="BE1" s="86"/>
     </row>
     <row r="2" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="52" t="s">
+      <c r="C2" s="73"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="52" t="s">
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="64"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="52" t="s">
+      <c r="K2" s="69"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="53" t="s">
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="64"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="52" t="s">
+      <c r="S2" s="69"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="52" t="s">
+      <c r="V2" s="73"/>
+      <c r="W2" s="73"/>
+      <c r="X2" s="73"/>
+      <c r="Y2" s="79"/>
+      <c r="Z2" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="52" t="s">
+      <c r="AA2" s="69"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
-      <c r="AF2" s="53"/>
-      <c r="AG2" s="54"/>
-      <c r="AH2" s="52" t="s">
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="73"/>
+      <c r="AF2" s="73"/>
+      <c r="AG2" s="79"/>
+      <c r="AH2" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="AI2" s="64"/>
-      <c r="AJ2" s="65"/>
-      <c r="AK2" s="52" t="s">
+      <c r="AI2" s="69"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="52" t="s">
+      <c r="AL2" s="73"/>
+      <c r="AM2" s="73"/>
+      <c r="AN2" s="73"/>
+      <c r="AO2" s="79"/>
+      <c r="AP2" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="AQ2" s="64"/>
-      <c r="AR2" s="65"/>
-      <c r="AS2" s="52" t="s">
+      <c r="AQ2" s="69"/>
+      <c r="AR2" s="54"/>
+      <c r="AS2" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="AT2" s="53"/>
-      <c r="AU2" s="53"/>
-      <c r="AV2" s="53"/>
-      <c r="AW2" s="54"/>
-      <c r="AX2" s="52" t="s">
+      <c r="AT2" s="73"/>
+      <c r="AU2" s="73"/>
+      <c r="AV2" s="73"/>
+      <c r="AW2" s="79"/>
+      <c r="AX2" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="AY2" s="64"/>
-      <c r="AZ2" s="65"/>
-      <c r="BA2" s="52" t="s">
+      <c r="AY2" s="69"/>
+      <c r="AZ2" s="54"/>
+      <c r="BA2" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="BB2" s="53"/>
-      <c r="BC2" s="53"/>
-      <c r="BD2" s="53"/>
-      <c r="BE2" s="54"/>
+      <c r="BB2" s="73"/>
+      <c r="BC2" s="73"/>
+      <c r="BD2" s="73"/>
+      <c r="BE2" s="79"/>
     </row>
     <row r="3" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A3" s="62"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="68"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="57"/>
-      <c r="Z3" s="66"/>
-      <c r="AA3" s="67"/>
-      <c r="AB3" s="68"/>
-      <c r="AC3" s="55"/>
-      <c r="AD3" s="56"/>
-      <c r="AE3" s="56"/>
-      <c r="AF3" s="56"/>
-      <c r="AG3" s="57"/>
-      <c r="AH3" s="66"/>
-      <c r="AI3" s="67"/>
-      <c r="AJ3" s="68"/>
-      <c r="AK3" s="55"/>
-      <c r="AL3" s="56"/>
-      <c r="AM3" s="56"/>
-      <c r="AN3" s="56"/>
-      <c r="AO3" s="57"/>
-      <c r="AP3" s="66"/>
-      <c r="AQ3" s="67"/>
-      <c r="AR3" s="68"/>
-      <c r="AS3" s="55"/>
-      <c r="AT3" s="56"/>
-      <c r="AU3" s="56"/>
-      <c r="AV3" s="56"/>
-      <c r="AW3" s="57"/>
-      <c r="AX3" s="66"/>
-      <c r="AY3" s="67"/>
-      <c r="AZ3" s="68"/>
-      <c r="BA3" s="55"/>
-      <c r="BB3" s="56"/>
-      <c r="BC3" s="56"/>
-      <c r="BD3" s="56"/>
-      <c r="BE3" s="57"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="75"/>
+      <c r="O3" s="75"/>
+      <c r="P3" s="75"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="56"/>
+      <c r="U3" s="77"/>
+      <c r="V3" s="75"/>
+      <c r="W3" s="75"/>
+      <c r="X3" s="75"/>
+      <c r="Y3" s="80"/>
+      <c r="Z3" s="72"/>
+      <c r="AA3" s="68"/>
+      <c r="AB3" s="56"/>
+      <c r="AC3" s="77"/>
+      <c r="AD3" s="75"/>
+      <c r="AE3" s="75"/>
+      <c r="AF3" s="75"/>
+      <c r="AG3" s="80"/>
+      <c r="AH3" s="72"/>
+      <c r="AI3" s="68"/>
+      <c r="AJ3" s="56"/>
+      <c r="AK3" s="77"/>
+      <c r="AL3" s="75"/>
+      <c r="AM3" s="75"/>
+      <c r="AN3" s="75"/>
+      <c r="AO3" s="80"/>
+      <c r="AP3" s="72"/>
+      <c r="AQ3" s="68"/>
+      <c r="AR3" s="56"/>
+      <c r="AS3" s="77"/>
+      <c r="AT3" s="75"/>
+      <c r="AU3" s="75"/>
+      <c r="AV3" s="75"/>
+      <c r="AW3" s="80"/>
+      <c r="AX3" s="72"/>
+      <c r="AY3" s="68"/>
+      <c r="AZ3" s="56"/>
+      <c r="BA3" s="77"/>
+      <c r="BB3" s="75"/>
+      <c r="BC3" s="75"/>
+      <c r="BD3" s="75"/>
+      <c r="BE3" s="80"/>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
-      <c r="B4" s="53" t="s">
+      <c r="A4" s="88"/>
+      <c r="B4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="64" t="s">
+      <c r="F4" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="64" t="s">
+      <c r="G4" s="78"/>
+      <c r="H4" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="83"/>
-      <c r="J4" s="86" t="s">
+      <c r="I4" s="63"/>
+      <c r="J4" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="89" t="s">
+      <c r="K4" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="83" t="s">
+      <c r="L4" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="73" t="s">
+      <c r="M4" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="89" t="s">
+      <c r="N4" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="89"/>
-      <c r="P4" s="89" t="s">
+      <c r="O4" s="60"/>
+      <c r="P4" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="73" t="s">
+      <c r="Q4" s="54"/>
+      <c r="R4" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="S4" s="89" t="s">
+      <c r="S4" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="T4" s="83" t="s">
+      <c r="T4" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="U4" s="73" t="s">
+      <c r="U4" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="V4" s="89" t="s">
+      <c r="V4" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="W4" s="64"/>
-      <c r="X4" s="89" t="s">
+      <c r="W4" s="69"/>
+      <c r="X4" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="Y4" s="65"/>
-      <c r="Z4" s="86" t="s">
+      <c r="Y4" s="54"/>
+      <c r="Z4" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="AA4" s="89" t="s">
+      <c r="AA4" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="AB4" s="83" t="s">
+      <c r="AB4" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="AC4" s="73" t="s">
+      <c r="AC4" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="AD4" s="89" t="s">
+      <c r="AD4" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="AE4" s="64"/>
-      <c r="AF4" s="89" t="s">
+      <c r="AE4" s="69"/>
+      <c r="AF4" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="AG4" s="65"/>
-      <c r="AH4" s="73" t="s">
+      <c r="AG4" s="54"/>
+      <c r="AH4" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="AI4" s="89" t="s">
+      <c r="AI4" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="83" t="s">
+      <c r="AJ4" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="73" t="s">
+      <c r="AK4" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="AL4" s="89" t="s">
+      <c r="AL4" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="AM4" s="64"/>
-      <c r="AN4" s="89" t="s">
+      <c r="AM4" s="69"/>
+      <c r="AN4" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="AO4" s="65"/>
-      <c r="AP4" s="73" t="s">
+      <c r="AO4" s="54"/>
+      <c r="AP4" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="AQ4" s="89" t="s">
+      <c r="AQ4" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="AR4" s="83" t="s">
+      <c r="AR4" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="AS4" s="73" t="s">
+      <c r="AS4" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="AT4" s="89" t="s">
+      <c r="AT4" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="AU4" s="64"/>
-      <c r="AV4" s="89" t="s">
+      <c r="AU4" s="69"/>
+      <c r="AV4" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="AW4" s="65"/>
-      <c r="AX4" s="86" t="s">
+      <c r="AW4" s="54"/>
+      <c r="AX4" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="AY4" s="89" t="s">
+      <c r="AY4" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="AZ4" s="83" t="s">
+      <c r="AZ4" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="BA4" s="90" t="s">
+      <c r="BA4" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="BB4" s="74" t="s">
+      <c r="BB4" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="BC4" s="77"/>
-      <c r="BD4" s="74" t="s">
+      <c r="BC4" s="67"/>
+      <c r="BD4" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="BE4" s="65"/>
+      <c r="BE4" s="54"/>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
-      <c r="B5" s="76"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="74"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="84"/>
-      <c r="U5" s="74"/>
-      <c r="V5" s="74"/>
-      <c r="W5" s="77"/>
-      <c r="X5" s="74"/>
-      <c r="Y5" s="78"/>
-      <c r="Z5" s="87"/>
-      <c r="AA5" s="81"/>
-      <c r="AB5" s="84"/>
-      <c r="AC5" s="74"/>
-      <c r="AD5" s="74"/>
-      <c r="AE5" s="77"/>
-      <c r="AF5" s="74"/>
-      <c r="AG5" s="78"/>
-      <c r="AH5" s="74"/>
-      <c r="AI5" s="81"/>
-      <c r="AJ5" s="84"/>
-      <c r="AK5" s="74"/>
-      <c r="AL5" s="81"/>
-      <c r="AM5" s="77"/>
-      <c r="AN5" s="74"/>
-      <c r="AO5" s="78"/>
-      <c r="AP5" s="74"/>
-      <c r="AQ5" s="81"/>
-      <c r="AR5" s="84"/>
-      <c r="AS5" s="74"/>
-      <c r="AT5" s="81"/>
-      <c r="AU5" s="77"/>
-      <c r="AV5" s="74"/>
-      <c r="AW5" s="78"/>
-      <c r="AX5" s="87"/>
-      <c r="AY5" s="81"/>
-      <c r="AZ5" s="84"/>
-      <c r="BA5" s="74"/>
-      <c r="BB5" s="81"/>
-      <c r="BC5" s="77"/>
-      <c r="BD5" s="74"/>
-      <c r="BE5" s="78"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="55"/>
+      <c r="R5" s="52"/>
+      <c r="S5" s="61"/>
+      <c r="T5" s="64"/>
+      <c r="U5" s="52"/>
+      <c r="V5" s="52"/>
+      <c r="W5" s="67"/>
+      <c r="X5" s="52"/>
+      <c r="Y5" s="55"/>
+      <c r="Z5" s="58"/>
+      <c r="AA5" s="61"/>
+      <c r="AB5" s="64"/>
+      <c r="AC5" s="52"/>
+      <c r="AD5" s="52"/>
+      <c r="AE5" s="67"/>
+      <c r="AF5" s="52"/>
+      <c r="AG5" s="55"/>
+      <c r="AH5" s="52"/>
+      <c r="AI5" s="61"/>
+      <c r="AJ5" s="64"/>
+      <c r="AK5" s="52"/>
+      <c r="AL5" s="61"/>
+      <c r="AM5" s="67"/>
+      <c r="AN5" s="52"/>
+      <c r="AO5" s="55"/>
+      <c r="AP5" s="52"/>
+      <c r="AQ5" s="61"/>
+      <c r="AR5" s="64"/>
+      <c r="AS5" s="52"/>
+      <c r="AT5" s="61"/>
+      <c r="AU5" s="67"/>
+      <c r="AV5" s="52"/>
+      <c r="AW5" s="55"/>
+      <c r="AX5" s="58"/>
+      <c r="AY5" s="61"/>
+      <c r="AZ5" s="64"/>
+      <c r="BA5" s="52"/>
+      <c r="BB5" s="61"/>
+      <c r="BC5" s="67"/>
+      <c r="BD5" s="52"/>
+      <c r="BE5" s="55"/>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
-      <c r="B6" s="76"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="74"/>
-      <c r="Q6" s="78"/>
-      <c r="R6" s="74"/>
-      <c r="S6" s="81"/>
-      <c r="T6" s="84"/>
-      <c r="U6" s="74"/>
-      <c r="V6" s="74"/>
-      <c r="W6" s="77"/>
-      <c r="X6" s="74"/>
-      <c r="Y6" s="78"/>
-      <c r="Z6" s="87"/>
-      <c r="AA6" s="81"/>
-      <c r="AB6" s="84"/>
-      <c r="AC6" s="74"/>
-      <c r="AD6" s="74"/>
-      <c r="AE6" s="77"/>
-      <c r="AF6" s="74"/>
-      <c r="AG6" s="78"/>
-      <c r="AH6" s="74"/>
-      <c r="AI6" s="81"/>
-      <c r="AJ6" s="84"/>
-      <c r="AK6" s="74"/>
-      <c r="AL6" s="81"/>
-      <c r="AM6" s="77"/>
-      <c r="AN6" s="74"/>
-      <c r="AO6" s="78"/>
-      <c r="AP6" s="74"/>
-      <c r="AQ6" s="81"/>
-      <c r="AR6" s="84"/>
-      <c r="AS6" s="74"/>
-      <c r="AT6" s="81"/>
-      <c r="AU6" s="77"/>
-      <c r="AV6" s="74"/>
-      <c r="AW6" s="78"/>
-      <c r="AX6" s="87"/>
-      <c r="AY6" s="81"/>
-      <c r="AZ6" s="84"/>
-      <c r="BA6" s="74"/>
-      <c r="BB6" s="81"/>
-      <c r="BC6" s="77"/>
-      <c r="BD6" s="74"/>
-      <c r="BE6" s="78"/>
+      <c r="A6" s="88"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="52"/>
+      <c r="Q6" s="55"/>
+      <c r="R6" s="52"/>
+      <c r="S6" s="61"/>
+      <c r="T6" s="64"/>
+      <c r="U6" s="52"/>
+      <c r="V6" s="52"/>
+      <c r="W6" s="67"/>
+      <c r="X6" s="52"/>
+      <c r="Y6" s="55"/>
+      <c r="Z6" s="58"/>
+      <c r="AA6" s="61"/>
+      <c r="AB6" s="64"/>
+      <c r="AC6" s="52"/>
+      <c r="AD6" s="52"/>
+      <c r="AE6" s="67"/>
+      <c r="AF6" s="52"/>
+      <c r="AG6" s="55"/>
+      <c r="AH6" s="52"/>
+      <c r="AI6" s="61"/>
+      <c r="AJ6" s="64"/>
+      <c r="AK6" s="52"/>
+      <c r="AL6" s="61"/>
+      <c r="AM6" s="67"/>
+      <c r="AN6" s="52"/>
+      <c r="AO6" s="55"/>
+      <c r="AP6" s="52"/>
+      <c r="AQ6" s="61"/>
+      <c r="AR6" s="64"/>
+      <c r="AS6" s="52"/>
+      <c r="AT6" s="61"/>
+      <c r="AU6" s="67"/>
+      <c r="AV6" s="52"/>
+      <c r="AW6" s="55"/>
+      <c r="AX6" s="58"/>
+      <c r="AY6" s="61"/>
+      <c r="AZ6" s="64"/>
+      <c r="BA6" s="52"/>
+      <c r="BB6" s="61"/>
+      <c r="BC6" s="67"/>
+      <c r="BD6" s="52"/>
+      <c r="BE6" s="55"/>
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A7" s="63"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="85"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="85"/>
-      <c r="M7" s="75"/>
-      <c r="N7" s="75"/>
-      <c r="O7" s="75"/>
-      <c r="P7" s="75"/>
-      <c r="Q7" s="68"/>
-      <c r="R7" s="75"/>
-      <c r="S7" s="82"/>
-      <c r="T7" s="85"/>
-      <c r="U7" s="75"/>
-      <c r="V7" s="75"/>
-      <c r="W7" s="67"/>
-      <c r="X7" s="75"/>
-      <c r="Y7" s="68"/>
-      <c r="Z7" s="88"/>
-      <c r="AA7" s="82"/>
-      <c r="AB7" s="85"/>
-      <c r="AC7" s="75"/>
-      <c r="AD7" s="75"/>
-      <c r="AE7" s="67"/>
-      <c r="AF7" s="75"/>
-      <c r="AG7" s="68"/>
-      <c r="AH7" s="75"/>
-      <c r="AI7" s="82"/>
-      <c r="AJ7" s="85"/>
-      <c r="AK7" s="75"/>
-      <c r="AL7" s="82"/>
-      <c r="AM7" s="67"/>
-      <c r="AN7" s="75"/>
-      <c r="AO7" s="68"/>
-      <c r="AP7" s="75"/>
-      <c r="AQ7" s="82"/>
-      <c r="AR7" s="85"/>
-      <c r="AS7" s="75"/>
-      <c r="AT7" s="82"/>
-      <c r="AU7" s="67"/>
-      <c r="AV7" s="75"/>
-      <c r="AW7" s="68"/>
-      <c r="AX7" s="88"/>
-      <c r="AY7" s="82"/>
-      <c r="AZ7" s="85"/>
-      <c r="BA7" s="75"/>
-      <c r="BB7" s="82"/>
-      <c r="BC7" s="67"/>
-      <c r="BD7" s="75"/>
-      <c r="BE7" s="68"/>
+      <c r="A7" s="89"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="53"/>
+      <c r="S7" s="62"/>
+      <c r="T7" s="65"/>
+      <c r="U7" s="53"/>
+      <c r="V7" s="53"/>
+      <c r="W7" s="68"/>
+      <c r="X7" s="53"/>
+      <c r="Y7" s="56"/>
+      <c r="Z7" s="59"/>
+      <c r="AA7" s="62"/>
+      <c r="AB7" s="65"/>
+      <c r="AC7" s="53"/>
+      <c r="AD7" s="53"/>
+      <c r="AE7" s="68"/>
+      <c r="AF7" s="53"/>
+      <c r="AG7" s="56"/>
+      <c r="AH7" s="53"/>
+      <c r="AI7" s="62"/>
+      <c r="AJ7" s="65"/>
+      <c r="AK7" s="53"/>
+      <c r="AL7" s="62"/>
+      <c r="AM7" s="68"/>
+      <c r="AN7" s="53"/>
+      <c r="AO7" s="56"/>
+      <c r="AP7" s="53"/>
+      <c r="AQ7" s="62"/>
+      <c r="AR7" s="65"/>
+      <c r="AS7" s="53"/>
+      <c r="AT7" s="62"/>
+      <c r="AU7" s="68"/>
+      <c r="AV7" s="53"/>
+      <c r="AW7" s="56"/>
+      <c r="AX7" s="59"/>
+      <c r="AY7" s="62"/>
+      <c r="AZ7" s="65"/>
+      <c r="BA7" s="53"/>
+      <c r="BB7" s="62"/>
+      <c r="BC7" s="68"/>
+      <c r="BD7" s="53"/>
+      <c r="BE7" s="56"/>
     </row>
     <row r="8" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A8" s="28"/>
@@ -5753,26 +5753,48 @@
     <sortCondition descending="1" ref="K23"/>
   </sortState>
   <mergeCells count="78">
-    <mergeCell ref="BD4:BD7"/>
-    <mergeCell ref="BE4:BE7"/>
-    <mergeCell ref="AX4:AX7"/>
-    <mergeCell ref="AY4:AY7"/>
-    <mergeCell ref="AZ4:AZ7"/>
-    <mergeCell ref="BA4:BA7"/>
-    <mergeCell ref="BB4:BB7"/>
-    <mergeCell ref="BC4:BC7"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="AL4:AL7"/>
-    <mergeCell ref="AM4:AM7"/>
-    <mergeCell ref="AN4:AN7"/>
-    <mergeCell ref="AO4:AO7"/>
-    <mergeCell ref="AP4:AP7"/>
-    <mergeCell ref="AQ4:AQ7"/>
-    <mergeCell ref="AR4:AR7"/>
-    <mergeCell ref="AS4:AS7"/>
-    <mergeCell ref="AT4:AT7"/>
-    <mergeCell ref="AU4:AU7"/>
-    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="BA2:BE3"/>
+    <mergeCell ref="AX1:BE1"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E2:I3"/>
+    <mergeCell ref="J2:L3"/>
+    <mergeCell ref="M2:Q3"/>
+    <mergeCell ref="R2:T3"/>
+    <mergeCell ref="U2:Y3"/>
+    <mergeCell ref="Z2:AB3"/>
+    <mergeCell ref="AC2:AG3"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="R1:Y1"/>
+    <mergeCell ref="Z1:AG1"/>
+    <mergeCell ref="AH1:AN1"/>
+    <mergeCell ref="AH2:AJ3"/>
+    <mergeCell ref="AK2:AO3"/>
+    <mergeCell ref="AP2:AR3"/>
+    <mergeCell ref="AS2:AW3"/>
+    <mergeCell ref="AP1:AV1"/>
+    <mergeCell ref="AX2:AZ3"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="Y4:Y7"/>
+    <mergeCell ref="N4:N7"/>
+    <mergeCell ref="O4:O7"/>
+    <mergeCell ref="P4:P7"/>
+    <mergeCell ref="Q4:Q7"/>
+    <mergeCell ref="R4:R7"/>
+    <mergeCell ref="S4:S7"/>
+    <mergeCell ref="T4:T7"/>
     <mergeCell ref="U4:U7"/>
     <mergeCell ref="V4:V7"/>
     <mergeCell ref="W4:W7"/>
@@ -5789,48 +5811,26 @@
     <mergeCell ref="AH4:AH7"/>
     <mergeCell ref="AI4:AI7"/>
     <mergeCell ref="AJ4:AJ7"/>
-    <mergeCell ref="P4:P7"/>
-    <mergeCell ref="Q4:Q7"/>
-    <mergeCell ref="R4:R7"/>
-    <mergeCell ref="S4:S7"/>
-    <mergeCell ref="T4:T7"/>
-    <mergeCell ref="AX2:AZ3"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="Y4:Y7"/>
-    <mergeCell ref="N4:N7"/>
-    <mergeCell ref="O4:O7"/>
-    <mergeCell ref="AH2:AJ3"/>
-    <mergeCell ref="AK2:AO3"/>
-    <mergeCell ref="AP2:AR3"/>
-    <mergeCell ref="AS2:AW3"/>
-    <mergeCell ref="AP1:AV1"/>
-    <mergeCell ref="BA2:BE3"/>
-    <mergeCell ref="AX1:BE1"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:D3"/>
-    <mergeCell ref="E2:I3"/>
-    <mergeCell ref="J2:L3"/>
-    <mergeCell ref="M2:Q3"/>
-    <mergeCell ref="R2:T3"/>
-    <mergeCell ref="U2:Y3"/>
-    <mergeCell ref="Z2:AB3"/>
-    <mergeCell ref="AC2:AG3"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:Y1"/>
-    <mergeCell ref="Z1:AG1"/>
-    <mergeCell ref="AH1:AN1"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="AL4:AL7"/>
+    <mergeCell ref="AM4:AM7"/>
+    <mergeCell ref="AN4:AN7"/>
+    <mergeCell ref="AO4:AO7"/>
+    <mergeCell ref="AP4:AP7"/>
+    <mergeCell ref="AQ4:AQ7"/>
+    <mergeCell ref="AR4:AR7"/>
+    <mergeCell ref="AS4:AS7"/>
+    <mergeCell ref="AT4:AT7"/>
+    <mergeCell ref="AU4:AU7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="BD4:BD7"/>
+    <mergeCell ref="BE4:BE7"/>
+    <mergeCell ref="AX4:AX7"/>
+    <mergeCell ref="AY4:AY7"/>
+    <mergeCell ref="AZ4:AZ7"/>
+    <mergeCell ref="BA4:BA7"/>
+    <mergeCell ref="BB4:BB7"/>
+    <mergeCell ref="BC4:BC7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Moved shiny app to new project
</commit_message>
<xml_diff>
--- a/Conception rates by age and country.xlsx
+++ b/Conception rates by age and country.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Under 16" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,10 @@
     <sheet name="Under 20" sheetId="5" r:id="rId3"/>
     <sheet name="Age 18-19" sheetId="3" r:id="rId4"/>
     <sheet name="Calcs and data insert" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="Table1Data">[1]table1Data!$A$1:$IV$65536</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="22">
   <si>
     <t>Country</t>
   </si>
@@ -120,6 +121,9 @@
   <si>
     <t>USA</t>
   </si>
+  <si>
+    <t>Conceptions to under 18s</t>
+  </si>
 </sst>
 </file>
 
@@ -173,12 +177,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="14">
@@ -339,7 +349,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -454,20 +464,107 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -481,96 +578,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma 2" xfId="1"/>
@@ -2367,7 +2381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2831,7 +2845,7 @@
     <sortCondition descending="1" ref="L9:L24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2840,10 +2854,10 @@
   <dimension ref="A1:AG30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE3" sqref="AE3"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3309,89 +3323,89 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:33" s="91" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="91">
         <v>71</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="91">
         <v>74</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="91">
         <v>74.8</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="91">
         <v>74.599999999999994</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="91">
         <v>73.2</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="92">
         <v>70.599999999999994</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="92">
         <v>69.7</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="92">
         <v>69.099999999999994</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="92">
         <v>64.400000000000006</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="92">
         <v>60.7</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="92">
         <v>56.9</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="92">
         <v>54.2</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="92">
         <v>50.8</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="92">
         <v>48.4</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="92">
         <v>44.4</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="Q6" s="92">
         <v>42</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6" s="92">
         <v>40.5</v>
       </c>
-      <c r="S6" s="1">
+      <c r="S6" s="92">
         <v>39.200000000000003</v>
       </c>
-      <c r="T6" s="1">
+      <c r="T6" s="92">
         <v>37.799999999999997</v>
       </c>
-      <c r="U6" s="1">
+      <c r="U6" s="92">
         <v>38.5</v>
       </c>
-      <c r="V6" s="1">
+      <c r="V6" s="92">
         <v>38.1</v>
       </c>
-      <c r="W6" s="1">
+      <c r="W6" s="92">
         <v>37</v>
       </c>
-      <c r="X6" s="1">
+      <c r="X6" s="92">
         <v>34.1</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="Y6" s="92">
         <v>30.3</v>
       </c>
-      <c r="Z6" s="1">
+      <c r="Z6" s="92">
         <v>26.7</v>
       </c>
-      <c r="AA6" s="1">
+      <c r="AA6" s="92">
         <v>24</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AB6" s="92">
         <v>20.8</v>
       </c>
     </row>
@@ -3474,10 +3488,10 @@
   <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE5" sqref="AE5"/>
+      <selection pane="bottomRight" activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3832,89 +3846,89 @@
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:33" s="91" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="91">
         <v>93.7</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="91">
         <v>98</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="91">
         <v>100.4</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="91">
         <v>102.4</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="91">
         <v>99.5</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="92">
         <v>95.7</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="92">
         <v>92.8</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="92">
         <v>89.4</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="92">
         <v>85.3</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="92">
         <v>81.8</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="92">
         <v>78.3</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="92">
         <v>76.400000000000006</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="92">
         <v>73.5</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="92">
         <v>71.5</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="92">
         <v>67.5</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="Q6" s="92">
         <v>63.7</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6" s="92">
         <v>61.3</v>
       </c>
-      <c r="S6" s="1">
+      <c r="S6" s="92">
         <v>59.6</v>
       </c>
-      <c r="T6" s="1">
+      <c r="T6" s="92">
         <v>58.3</v>
       </c>
-      <c r="U6" s="1">
+      <c r="U6" s="92">
         <v>60</v>
       </c>
-      <c r="V6" s="1">
+      <c r="V6" s="92">
         <v>59.9</v>
       </c>
-      <c r="W6" s="1">
+      <c r="W6" s="92">
         <v>58.4</v>
       </c>
-      <c r="X6" s="1">
+      <c r="X6" s="92">
         <v>54.6</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="Y6" s="92">
         <v>49.4</v>
       </c>
-      <c r="Z6" s="1">
+      <c r="Z6" s="92">
         <v>53.3</v>
       </c>
-      <c r="AA6" s="1">
+      <c r="AA6" s="92">
         <v>49.1</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AB6" s="92">
         <v>44.1</v>
       </c>
     </row>
@@ -3923,7 +3937,7 @@
     <sortCondition descending="1" ref="I11:I32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3935,7 +3949,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC6" sqref="AC6"/>
+      <selection pane="bottomRight" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4230,89 +4244,89 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:33" s="91" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="91">
         <v>160.5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="91">
         <v>164.7</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="91">
         <v>167.8</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="91">
         <v>173.3</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="91">
         <v>175</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="91">
         <v>172</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="91">
         <v>166.6</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="91">
         <v>161.80000000000001</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="91">
         <v>155.30000000000001</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="91">
         <v>150.9</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="91">
         <v>146</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="91">
         <v>141.69999999999999</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="91">
         <v>138</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="91">
         <v>135.9</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="91">
         <v>130.9</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="91">
         <v>124.4</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="91">
         <v>119.9</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="91">
         <v>117.5</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="91">
         <v>116</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="91">
         <v>119.9</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="91">
         <v>119.2</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="91">
         <v>113.8</v>
       </c>
-      <c r="X6">
+      <c r="X6" s="91">
         <v>105.9</v>
       </c>
-      <c r="Y6">
+      <c r="Y6" s="91">
         <v>96.7</v>
       </c>
-      <c r="Z6">
+      <c r="Z6" s="91">
         <v>89.2</v>
       </c>
-      <c r="AA6">
+      <c r="AA6" s="91">
         <v>83.2</v>
       </c>
-      <c r="AB6">
+      <c r="AB6" s="91">
         <v>76.099999999999994</v>
       </c>
     </row>
@@ -4325,8 +4339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AT9" sqref="AT9"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4335,544 +4349,544 @@
       <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="85">
+      <c r="B1" s="59">
         <v>2015</v>
       </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="84">
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="58">
         <v>2014</v>
       </c>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="85"/>
-      <c r="O1" s="85"/>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="85">
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="59">
         <v>2013</v>
       </c>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
-      <c r="U1" s="85"/>
-      <c r="V1" s="85"/>
-      <c r="W1" s="85"/>
-      <c r="X1" s="85"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="84">
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="58">
         <v>2012</v>
       </c>
-      <c r="AA1" s="85"/>
-      <c r="AB1" s="85"/>
-      <c r="AC1" s="85"/>
-      <c r="AD1" s="85"/>
-      <c r="AE1" s="85"/>
-      <c r="AF1" s="85"/>
-      <c r="AG1" s="86"/>
-      <c r="AH1" s="81">
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="59"/>
+      <c r="AF1" s="59"/>
+      <c r="AG1" s="60"/>
+      <c r="AH1" s="70">
         <v>2011</v>
       </c>
-      <c r="AI1" s="82"/>
-      <c r="AJ1" s="82"/>
-      <c r="AK1" s="82"/>
-      <c r="AL1" s="82"/>
-      <c r="AM1" s="82"/>
-      <c r="AN1" s="83"/>
+      <c r="AI1" s="71"/>
+      <c r="AJ1" s="71"/>
+      <c r="AK1" s="71"/>
+      <c r="AL1" s="71"/>
+      <c r="AM1" s="71"/>
+      <c r="AN1" s="72"/>
       <c r="AO1" s="27"/>
-      <c r="AP1" s="81">
+      <c r="AP1" s="70">
         <v>2010</v>
       </c>
-      <c r="AQ1" s="82"/>
-      <c r="AR1" s="82"/>
-      <c r="AS1" s="82"/>
-      <c r="AT1" s="82"/>
-      <c r="AU1" s="82"/>
-      <c r="AV1" s="83"/>
+      <c r="AQ1" s="71"/>
+      <c r="AR1" s="71"/>
+      <c r="AS1" s="71"/>
+      <c r="AT1" s="71"/>
+      <c r="AU1" s="71"/>
+      <c r="AV1" s="72"/>
       <c r="AW1" s="27"/>
-      <c r="AX1" s="84">
+      <c r="AX1" s="58">
         <v>2009</v>
       </c>
-      <c r="AY1" s="85"/>
-      <c r="AZ1" s="85"/>
-      <c r="BA1" s="85"/>
-      <c r="BB1" s="85"/>
-      <c r="BC1" s="85"/>
-      <c r="BD1" s="85"/>
-      <c r="BE1" s="86"/>
+      <c r="AY1" s="59"/>
+      <c r="AZ1" s="59"/>
+      <c r="BA1" s="59"/>
+      <c r="BB1" s="59"/>
+      <c r="BC1" s="59"/>
+      <c r="BD1" s="59"/>
+      <c r="BE1" s="60"/>
     </row>
     <row r="2" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="71" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="71" t="s">
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="69"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="71" t="s">
+      <c r="K2" s="64"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="73" t="s">
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="69"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="71" t="s">
+      <c r="S2" s="64"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="73"/>
-      <c r="W2" s="73"/>
-      <c r="X2" s="73"/>
-      <c r="Y2" s="79"/>
-      <c r="Z2" s="71" t="s">
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="AA2" s="69"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="71" t="s">
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="73"/>
-      <c r="AF2" s="73"/>
-      <c r="AG2" s="79"/>
-      <c r="AH2" s="71" t="s">
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="53"/>
+      <c r="AF2" s="53"/>
+      <c r="AG2" s="54"/>
+      <c r="AH2" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="AI2" s="69"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="71" t="s">
+      <c r="AI2" s="64"/>
+      <c r="AJ2" s="65"/>
+      <c r="AK2" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="AL2" s="73"/>
-      <c r="AM2" s="73"/>
-      <c r="AN2" s="73"/>
-      <c r="AO2" s="79"/>
-      <c r="AP2" s="71" t="s">
+      <c r="AL2" s="53"/>
+      <c r="AM2" s="53"/>
+      <c r="AN2" s="53"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="AQ2" s="69"/>
-      <c r="AR2" s="54"/>
-      <c r="AS2" s="71" t="s">
+      <c r="AQ2" s="64"/>
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="AT2" s="73"/>
-      <c r="AU2" s="73"/>
-      <c r="AV2" s="73"/>
-      <c r="AW2" s="79"/>
-      <c r="AX2" s="71" t="s">
+      <c r="AT2" s="53"/>
+      <c r="AU2" s="53"/>
+      <c r="AV2" s="53"/>
+      <c r="AW2" s="54"/>
+      <c r="AX2" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="AY2" s="69"/>
-      <c r="AZ2" s="54"/>
-      <c r="BA2" s="71" t="s">
+      <c r="AY2" s="64"/>
+      <c r="AZ2" s="65"/>
+      <c r="BA2" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="BB2" s="73"/>
-      <c r="BC2" s="73"/>
-      <c r="BD2" s="73"/>
-      <c r="BE2" s="79"/>
+      <c r="BB2" s="53"/>
+      <c r="BC2" s="53"/>
+      <c r="BD2" s="53"/>
+      <c r="BE2" s="54"/>
     </row>
     <row r="3" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A3" s="88"/>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="77"/>
-      <c r="V3" s="75"/>
-      <c r="W3" s="75"/>
-      <c r="X3" s="75"/>
-      <c r="Y3" s="80"/>
-      <c r="Z3" s="72"/>
-      <c r="AA3" s="68"/>
-      <c r="AB3" s="56"/>
-      <c r="AC3" s="77"/>
-      <c r="AD3" s="75"/>
-      <c r="AE3" s="75"/>
-      <c r="AF3" s="75"/>
-      <c r="AG3" s="80"/>
-      <c r="AH3" s="72"/>
-      <c r="AI3" s="68"/>
-      <c r="AJ3" s="56"/>
-      <c r="AK3" s="77"/>
-      <c r="AL3" s="75"/>
-      <c r="AM3" s="75"/>
-      <c r="AN3" s="75"/>
-      <c r="AO3" s="80"/>
-      <c r="AP3" s="72"/>
-      <c r="AQ3" s="68"/>
-      <c r="AR3" s="56"/>
-      <c r="AS3" s="77"/>
-      <c r="AT3" s="75"/>
-      <c r="AU3" s="75"/>
-      <c r="AV3" s="75"/>
-      <c r="AW3" s="80"/>
-      <c r="AX3" s="72"/>
-      <c r="AY3" s="68"/>
-      <c r="AZ3" s="56"/>
-      <c r="BA3" s="77"/>
-      <c r="BB3" s="75"/>
-      <c r="BC3" s="75"/>
-      <c r="BD3" s="75"/>
-      <c r="BE3" s="80"/>
+      <c r="A3" s="62"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="55"/>
+      <c r="V3" s="56"/>
+      <c r="W3" s="56"/>
+      <c r="X3" s="56"/>
+      <c r="Y3" s="57"/>
+      <c r="Z3" s="66"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="55"/>
+      <c r="AD3" s="56"/>
+      <c r="AE3" s="56"/>
+      <c r="AF3" s="56"/>
+      <c r="AG3" s="57"/>
+      <c r="AH3" s="66"/>
+      <c r="AI3" s="67"/>
+      <c r="AJ3" s="68"/>
+      <c r="AK3" s="55"/>
+      <c r="AL3" s="56"/>
+      <c r="AM3" s="56"/>
+      <c r="AN3" s="56"/>
+      <c r="AO3" s="57"/>
+      <c r="AP3" s="66"/>
+      <c r="AQ3" s="67"/>
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="55"/>
+      <c r="AT3" s="56"/>
+      <c r="AU3" s="56"/>
+      <c r="AV3" s="56"/>
+      <c r="AW3" s="57"/>
+      <c r="AX3" s="66"/>
+      <c r="AY3" s="67"/>
+      <c r="AZ3" s="68"/>
+      <c r="BA3" s="55"/>
+      <c r="BB3" s="56"/>
+      <c r="BC3" s="56"/>
+      <c r="BD3" s="56"/>
+      <c r="BE3" s="57"/>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A4" s="88"/>
-      <c r="B4" s="73" t="s">
+      <c r="A4" s="62"/>
+      <c r="B4" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="71" t="s">
+      <c r="E4" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="69" t="s">
+      <c r="F4" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="78"/>
-      <c r="H4" s="69" t="s">
+      <c r="G4" s="80"/>
+      <c r="H4" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="63"/>
-      <c r="J4" s="57" t="s">
+      <c r="I4" s="83"/>
+      <c r="J4" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="60" t="s">
+      <c r="K4" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="63" t="s">
+      <c r="L4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="70" t="s">
+      <c r="M4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="60" t="s">
+      <c r="N4" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60" t="s">
+      <c r="O4" s="89"/>
+      <c r="P4" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="70" t="s">
+      <c r="Q4" s="65"/>
+      <c r="R4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="S4" s="60" t="s">
+      <c r="S4" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="T4" s="63" t="s">
+      <c r="T4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="U4" s="70" t="s">
+      <c r="U4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="V4" s="60" t="s">
+      <c r="V4" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="W4" s="69"/>
-      <c r="X4" s="60" t="s">
+      <c r="W4" s="64"/>
+      <c r="X4" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="Y4" s="54"/>
-      <c r="Z4" s="57" t="s">
+      <c r="Y4" s="65"/>
+      <c r="Z4" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="AA4" s="60" t="s">
+      <c r="AA4" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="AB4" s="63" t="s">
+      <c r="AB4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="AC4" s="70" t="s">
+      <c r="AC4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="AD4" s="60" t="s">
+      <c r="AD4" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="AE4" s="69"/>
-      <c r="AF4" s="60" t="s">
+      <c r="AE4" s="64"/>
+      <c r="AF4" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="AG4" s="54"/>
-      <c r="AH4" s="70" t="s">
+      <c r="AG4" s="65"/>
+      <c r="AH4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="AI4" s="60" t="s">
+      <c r="AI4" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="63" t="s">
+      <c r="AJ4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="70" t="s">
+      <c r="AK4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="AL4" s="60" t="s">
+      <c r="AL4" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="AM4" s="69"/>
-      <c r="AN4" s="60" t="s">
+      <c r="AM4" s="64"/>
+      <c r="AN4" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="AO4" s="54"/>
-      <c r="AP4" s="70" t="s">
+      <c r="AO4" s="65"/>
+      <c r="AP4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="AQ4" s="60" t="s">
+      <c r="AQ4" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="AR4" s="63" t="s">
+      <c r="AR4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="AS4" s="70" t="s">
+      <c r="AS4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="AT4" s="60" t="s">
+      <c r="AT4" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="AU4" s="69"/>
-      <c r="AV4" s="60" t="s">
+      <c r="AU4" s="64"/>
+      <c r="AV4" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="AW4" s="54"/>
-      <c r="AX4" s="57" t="s">
+      <c r="AW4" s="65"/>
+      <c r="AX4" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="AY4" s="60" t="s">
+      <c r="AY4" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="AZ4" s="63" t="s">
+      <c r="AZ4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="BA4" s="66" t="s">
+      <c r="BA4" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="BB4" s="52" t="s">
+      <c r="BB4" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="BC4" s="67"/>
-      <c r="BD4" s="52" t="s">
+      <c r="BC4" s="77"/>
+      <c r="BD4" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="BE4" s="54"/>
+      <c r="BE4" s="65"/>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A5" s="88"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="55"/>
-      <c r="R5" s="52"/>
-      <c r="S5" s="61"/>
-      <c r="T5" s="64"/>
-      <c r="U5" s="52"/>
-      <c r="V5" s="52"/>
-      <c r="W5" s="67"/>
-      <c r="X5" s="52"/>
-      <c r="Y5" s="55"/>
-      <c r="Z5" s="58"/>
-      <c r="AA5" s="61"/>
-      <c r="AB5" s="64"/>
-      <c r="AC5" s="52"/>
-      <c r="AD5" s="52"/>
-      <c r="AE5" s="67"/>
-      <c r="AF5" s="52"/>
-      <c r="AG5" s="55"/>
-      <c r="AH5" s="52"/>
-      <c r="AI5" s="61"/>
-      <c r="AJ5" s="64"/>
-      <c r="AK5" s="52"/>
-      <c r="AL5" s="61"/>
-      <c r="AM5" s="67"/>
-      <c r="AN5" s="52"/>
-      <c r="AO5" s="55"/>
-      <c r="AP5" s="52"/>
-      <c r="AQ5" s="61"/>
-      <c r="AR5" s="64"/>
-      <c r="AS5" s="52"/>
-      <c r="AT5" s="61"/>
-      <c r="AU5" s="67"/>
-      <c r="AV5" s="52"/>
-      <c r="AW5" s="55"/>
-      <c r="AX5" s="58"/>
-      <c r="AY5" s="61"/>
-      <c r="AZ5" s="64"/>
-      <c r="BA5" s="52"/>
-      <c r="BB5" s="61"/>
-      <c r="BC5" s="67"/>
-      <c r="BD5" s="52"/>
-      <c r="BE5" s="55"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="74"/>
+      <c r="S5" s="81"/>
+      <c r="T5" s="84"/>
+      <c r="U5" s="74"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="77"/>
+      <c r="X5" s="74"/>
+      <c r="Y5" s="78"/>
+      <c r="Z5" s="87"/>
+      <c r="AA5" s="81"/>
+      <c r="AB5" s="84"/>
+      <c r="AC5" s="74"/>
+      <c r="AD5" s="74"/>
+      <c r="AE5" s="77"/>
+      <c r="AF5" s="74"/>
+      <c r="AG5" s="78"/>
+      <c r="AH5" s="74"/>
+      <c r="AI5" s="81"/>
+      <c r="AJ5" s="84"/>
+      <c r="AK5" s="74"/>
+      <c r="AL5" s="81"/>
+      <c r="AM5" s="77"/>
+      <c r="AN5" s="74"/>
+      <c r="AO5" s="78"/>
+      <c r="AP5" s="74"/>
+      <c r="AQ5" s="81"/>
+      <c r="AR5" s="84"/>
+      <c r="AS5" s="74"/>
+      <c r="AT5" s="81"/>
+      <c r="AU5" s="77"/>
+      <c r="AV5" s="74"/>
+      <c r="AW5" s="78"/>
+      <c r="AX5" s="87"/>
+      <c r="AY5" s="81"/>
+      <c r="AZ5" s="84"/>
+      <c r="BA5" s="74"/>
+      <c r="BB5" s="81"/>
+      <c r="BC5" s="77"/>
+      <c r="BD5" s="74"/>
+      <c r="BE5" s="78"/>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A6" s="88"/>
-      <c r="B6" s="74"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="55"/>
-      <c r="R6" s="52"/>
-      <c r="S6" s="61"/>
-      <c r="T6" s="64"/>
-      <c r="U6" s="52"/>
-      <c r="V6" s="52"/>
-      <c r="W6" s="67"/>
-      <c r="X6" s="52"/>
-      <c r="Y6" s="55"/>
-      <c r="Z6" s="58"/>
-      <c r="AA6" s="61"/>
-      <c r="AB6" s="64"/>
-      <c r="AC6" s="52"/>
-      <c r="AD6" s="52"/>
-      <c r="AE6" s="67"/>
-      <c r="AF6" s="52"/>
-      <c r="AG6" s="55"/>
-      <c r="AH6" s="52"/>
-      <c r="AI6" s="61"/>
-      <c r="AJ6" s="64"/>
-      <c r="AK6" s="52"/>
-      <c r="AL6" s="61"/>
-      <c r="AM6" s="67"/>
-      <c r="AN6" s="52"/>
-      <c r="AO6" s="55"/>
-      <c r="AP6" s="52"/>
-      <c r="AQ6" s="61"/>
-      <c r="AR6" s="64"/>
-      <c r="AS6" s="52"/>
-      <c r="AT6" s="61"/>
-      <c r="AU6" s="67"/>
-      <c r="AV6" s="52"/>
-      <c r="AW6" s="55"/>
-      <c r="AX6" s="58"/>
-      <c r="AY6" s="61"/>
-      <c r="AZ6" s="64"/>
-      <c r="BA6" s="52"/>
-      <c r="BB6" s="61"/>
-      <c r="BC6" s="67"/>
-      <c r="BD6" s="52"/>
-      <c r="BE6" s="55"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="74"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="74"/>
+      <c r="S6" s="81"/>
+      <c r="T6" s="84"/>
+      <c r="U6" s="74"/>
+      <c r="V6" s="74"/>
+      <c r="W6" s="77"/>
+      <c r="X6" s="74"/>
+      <c r="Y6" s="78"/>
+      <c r="Z6" s="87"/>
+      <c r="AA6" s="81"/>
+      <c r="AB6" s="84"/>
+      <c r="AC6" s="74"/>
+      <c r="AD6" s="74"/>
+      <c r="AE6" s="77"/>
+      <c r="AF6" s="74"/>
+      <c r="AG6" s="78"/>
+      <c r="AH6" s="74"/>
+      <c r="AI6" s="81"/>
+      <c r="AJ6" s="84"/>
+      <c r="AK6" s="74"/>
+      <c r="AL6" s="81"/>
+      <c r="AM6" s="77"/>
+      <c r="AN6" s="74"/>
+      <c r="AO6" s="78"/>
+      <c r="AP6" s="74"/>
+      <c r="AQ6" s="81"/>
+      <c r="AR6" s="84"/>
+      <c r="AS6" s="74"/>
+      <c r="AT6" s="81"/>
+      <c r="AU6" s="77"/>
+      <c r="AV6" s="74"/>
+      <c r="AW6" s="78"/>
+      <c r="AX6" s="87"/>
+      <c r="AY6" s="81"/>
+      <c r="AZ6" s="84"/>
+      <c r="BA6" s="74"/>
+      <c r="BB6" s="81"/>
+      <c r="BC6" s="77"/>
+      <c r="BD6" s="74"/>
+      <c r="BE6" s="78"/>
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A7" s="89"/>
-      <c r="B7" s="75"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="62"/>
-      <c r="T7" s="65"/>
-      <c r="U7" s="53"/>
-      <c r="V7" s="53"/>
-      <c r="W7" s="68"/>
-      <c r="X7" s="53"/>
-      <c r="Y7" s="56"/>
-      <c r="Z7" s="59"/>
-      <c r="AA7" s="62"/>
-      <c r="AB7" s="65"/>
-      <c r="AC7" s="53"/>
-      <c r="AD7" s="53"/>
-      <c r="AE7" s="68"/>
-      <c r="AF7" s="53"/>
-      <c r="AG7" s="56"/>
-      <c r="AH7" s="53"/>
-      <c r="AI7" s="62"/>
-      <c r="AJ7" s="65"/>
-      <c r="AK7" s="53"/>
-      <c r="AL7" s="62"/>
-      <c r="AM7" s="68"/>
-      <c r="AN7" s="53"/>
-      <c r="AO7" s="56"/>
-      <c r="AP7" s="53"/>
-      <c r="AQ7" s="62"/>
-      <c r="AR7" s="65"/>
-      <c r="AS7" s="53"/>
-      <c r="AT7" s="62"/>
-      <c r="AU7" s="68"/>
-      <c r="AV7" s="53"/>
-      <c r="AW7" s="56"/>
-      <c r="AX7" s="59"/>
-      <c r="AY7" s="62"/>
-      <c r="AZ7" s="65"/>
-      <c r="BA7" s="53"/>
-      <c r="BB7" s="62"/>
-      <c r="BC7" s="68"/>
-      <c r="BD7" s="53"/>
-      <c r="BE7" s="56"/>
+      <c r="A7" s="63"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="88"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="85"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="68"/>
+      <c r="R7" s="75"/>
+      <c r="S7" s="82"/>
+      <c r="T7" s="85"/>
+      <c r="U7" s="75"/>
+      <c r="V7" s="75"/>
+      <c r="W7" s="67"/>
+      <c r="X7" s="75"/>
+      <c r="Y7" s="68"/>
+      <c r="Z7" s="88"/>
+      <c r="AA7" s="82"/>
+      <c r="AB7" s="85"/>
+      <c r="AC7" s="75"/>
+      <c r="AD7" s="75"/>
+      <c r="AE7" s="67"/>
+      <c r="AF7" s="75"/>
+      <c r="AG7" s="68"/>
+      <c r="AH7" s="75"/>
+      <c r="AI7" s="82"/>
+      <c r="AJ7" s="85"/>
+      <c r="AK7" s="75"/>
+      <c r="AL7" s="82"/>
+      <c r="AM7" s="67"/>
+      <c r="AN7" s="75"/>
+      <c r="AO7" s="68"/>
+      <c r="AP7" s="75"/>
+      <c r="AQ7" s="82"/>
+      <c r="AR7" s="85"/>
+      <c r="AS7" s="75"/>
+      <c r="AT7" s="82"/>
+      <c r="AU7" s="67"/>
+      <c r="AV7" s="75"/>
+      <c r="AW7" s="68"/>
+      <c r="AX7" s="88"/>
+      <c r="AY7" s="82"/>
+      <c r="AZ7" s="85"/>
+      <c r="BA7" s="75"/>
+      <c r="BB7" s="82"/>
+      <c r="BC7" s="67"/>
+      <c r="BD7" s="75"/>
+      <c r="BE7" s="68"/>
     </row>
     <row r="8" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A8" s="28"/>
@@ -5753,6 +5767,68 @@
     <sortCondition descending="1" ref="K23"/>
   </sortState>
   <mergeCells count="78">
+    <mergeCell ref="BD4:BD7"/>
+    <mergeCell ref="BE4:BE7"/>
+    <mergeCell ref="AX4:AX7"/>
+    <mergeCell ref="AY4:AY7"/>
+    <mergeCell ref="AZ4:AZ7"/>
+    <mergeCell ref="BA4:BA7"/>
+    <mergeCell ref="BB4:BB7"/>
+    <mergeCell ref="BC4:BC7"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="AL4:AL7"/>
+    <mergeCell ref="AM4:AM7"/>
+    <mergeCell ref="AN4:AN7"/>
+    <mergeCell ref="AO4:AO7"/>
+    <mergeCell ref="AP4:AP7"/>
+    <mergeCell ref="AQ4:AQ7"/>
+    <mergeCell ref="AR4:AR7"/>
+    <mergeCell ref="AS4:AS7"/>
+    <mergeCell ref="AT4:AT7"/>
+    <mergeCell ref="AU4:AU7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="U4:U7"/>
+    <mergeCell ref="V4:V7"/>
+    <mergeCell ref="W4:W7"/>
+    <mergeCell ref="X4:X7"/>
+    <mergeCell ref="AK4:AK7"/>
+    <mergeCell ref="Z4:Z7"/>
+    <mergeCell ref="AA4:AA7"/>
+    <mergeCell ref="AB4:AB7"/>
+    <mergeCell ref="AC4:AC7"/>
+    <mergeCell ref="AD4:AD7"/>
+    <mergeCell ref="AE4:AE7"/>
+    <mergeCell ref="AF4:AF7"/>
+    <mergeCell ref="AG4:AG7"/>
+    <mergeCell ref="AH4:AH7"/>
+    <mergeCell ref="AI4:AI7"/>
+    <mergeCell ref="AJ4:AJ7"/>
+    <mergeCell ref="P4:P7"/>
+    <mergeCell ref="Q4:Q7"/>
+    <mergeCell ref="R4:R7"/>
+    <mergeCell ref="S4:S7"/>
+    <mergeCell ref="T4:T7"/>
+    <mergeCell ref="AX2:AZ3"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="Y4:Y7"/>
+    <mergeCell ref="N4:N7"/>
+    <mergeCell ref="O4:O7"/>
+    <mergeCell ref="AH2:AJ3"/>
+    <mergeCell ref="AK2:AO3"/>
+    <mergeCell ref="AP2:AR3"/>
+    <mergeCell ref="AS2:AW3"/>
+    <mergeCell ref="AP1:AV1"/>
     <mergeCell ref="BA2:BE3"/>
     <mergeCell ref="AX1:BE1"/>
     <mergeCell ref="A2:A7"/>
@@ -5769,69 +5845,101 @@
     <mergeCell ref="R1:Y1"/>
     <mergeCell ref="Z1:AG1"/>
     <mergeCell ref="AH1:AN1"/>
-    <mergeCell ref="AH2:AJ3"/>
-    <mergeCell ref="AK2:AO3"/>
-    <mergeCell ref="AP2:AR3"/>
-    <mergeCell ref="AS2:AW3"/>
-    <mergeCell ref="AP1:AV1"/>
-    <mergeCell ref="AX2:AZ3"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="Y4:Y7"/>
-    <mergeCell ref="N4:N7"/>
-    <mergeCell ref="O4:O7"/>
-    <mergeCell ref="P4:P7"/>
-    <mergeCell ref="Q4:Q7"/>
-    <mergeCell ref="R4:R7"/>
-    <mergeCell ref="S4:S7"/>
-    <mergeCell ref="T4:T7"/>
-    <mergeCell ref="U4:U7"/>
-    <mergeCell ref="V4:V7"/>
-    <mergeCell ref="W4:W7"/>
-    <mergeCell ref="X4:X7"/>
-    <mergeCell ref="AK4:AK7"/>
-    <mergeCell ref="Z4:Z7"/>
-    <mergeCell ref="AA4:AA7"/>
-    <mergeCell ref="AB4:AB7"/>
-    <mergeCell ref="AC4:AC7"/>
-    <mergeCell ref="AD4:AD7"/>
-    <mergeCell ref="AE4:AE7"/>
-    <mergeCell ref="AF4:AF7"/>
-    <mergeCell ref="AG4:AG7"/>
-    <mergeCell ref="AH4:AH7"/>
-    <mergeCell ref="AI4:AI7"/>
-    <mergeCell ref="AJ4:AJ7"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="AL4:AL7"/>
-    <mergeCell ref="AM4:AM7"/>
-    <mergeCell ref="AN4:AN7"/>
-    <mergeCell ref="AO4:AO7"/>
-    <mergeCell ref="AP4:AP7"/>
-    <mergeCell ref="AQ4:AQ7"/>
-    <mergeCell ref="AR4:AR7"/>
-    <mergeCell ref="AS4:AS7"/>
-    <mergeCell ref="AT4:AT7"/>
-    <mergeCell ref="AU4:AU7"/>
-    <mergeCell ref="AV4:AV7"/>
-    <mergeCell ref="BD4:BD7"/>
-    <mergeCell ref="BE4:BE7"/>
-    <mergeCell ref="AX4:AX7"/>
-    <mergeCell ref="AY4:AY7"/>
-    <mergeCell ref="AZ4:AZ7"/>
-    <mergeCell ref="BA4:BA7"/>
-    <mergeCell ref="BB4:BB7"/>
-    <mergeCell ref="BC4:BC7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="47">
+        <v>2001</v>
+      </c>
+      <c r="C1" s="47">
+        <v>2002</v>
+      </c>
+      <c r="D1" s="47">
+        <v>2003</v>
+      </c>
+      <c r="E1" s="47">
+        <v>2004</v>
+      </c>
+      <c r="F1" s="47">
+        <v>2005</v>
+      </c>
+      <c r="G1" s="47">
+        <v>2006</v>
+      </c>
+      <c r="H1" s="47">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="93">
+        <v>38461</v>
+      </c>
+      <c r="C2" s="93">
+        <v>39350</v>
+      </c>
+      <c r="D2" s="93">
+        <v>39553</v>
+      </c>
+      <c r="E2" s="93">
+        <v>39593</v>
+      </c>
+      <c r="F2" s="94">
+        <v>39804</v>
+      </c>
+      <c r="G2" s="94">
+        <v>39170</v>
+      </c>
+      <c r="H2" s="93">
+        <v>40366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="93">
+        <v>2529</v>
+      </c>
+      <c r="C3" s="93">
+        <v>2601</v>
+      </c>
+      <c r="D3" s="93">
+        <v>2609</v>
+      </c>
+      <c r="E3" s="93">
+        <v>2605</v>
+      </c>
+      <c r="F3" s="94">
+        <v>2521</v>
+      </c>
+      <c r="G3" s="94">
+        <v>2598</v>
+      </c>
+      <c r="H3" s="93">
+        <v>2622</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new idea - shiny Rmd to add to shiny server to redo synthetic control
</commit_message>
<xml_diff>
--- a/Conception rates by age and country.xlsx
+++ b/Conception rates by age and country.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2286432b\OneDrive - University of Glasgow\R Studio - home folder\teen-preg-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/a_baxter_1_research_gla_ac_uk/Documents/R Studio - home folder/teen-preg-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_2E4760DA000B1E54AFDAF35D778596A5BD5FBD80" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_2E4760DA000B1E54AFDAF35D778596A5BD5FBD80" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B0A46F46-86BE-4D9A-8822-CB85508D14C0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Under 16" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -468,24 +471,102 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -504,86 +585,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2868,7 +2871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3502,11 +3505,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2:AE2"/>
+      <selection pane="bottomRight" activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3714,7 +3717,7 @@
         <v>32.439142872564368</v>
       </c>
       <c r="AE2" s="1">
-        <v>31.6</v>
+        <v>31.7</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
@@ -4403,544 +4406,544 @@
       <c r="A1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="50">
+      <c r="B1" s="76">
         <v>2015</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="49">
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="75">
         <v>2014</v>
       </c>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="50">
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="76">
         <v>2013</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="49">
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="75">
         <v>2012</v>
       </c>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="50"/>
-      <c r="AC1" s="50"/>
-      <c r="AD1" s="50"/>
-      <c r="AE1" s="50"/>
-      <c r="AF1" s="50"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="61">
+      <c r="AA1" s="76"/>
+      <c r="AB1" s="76"/>
+      <c r="AC1" s="76"/>
+      <c r="AD1" s="76"/>
+      <c r="AE1" s="76"/>
+      <c r="AF1" s="76"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="72">
         <v>2011</v>
       </c>
-      <c r="AI1" s="62"/>
-      <c r="AJ1" s="62"/>
-      <c r="AK1" s="62"/>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="63"/>
+      <c r="AI1" s="73"/>
+      <c r="AJ1" s="73"/>
+      <c r="AK1" s="73"/>
+      <c r="AL1" s="73"/>
+      <c r="AM1" s="73"/>
+      <c r="AN1" s="74"/>
       <c r="AO1" s="21"/>
-      <c r="AP1" s="61">
+      <c r="AP1" s="72">
         <v>2010</v>
       </c>
-      <c r="AQ1" s="62"/>
-      <c r="AR1" s="62"/>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="62"/>
-      <c r="AU1" s="62"/>
-      <c r="AV1" s="63"/>
+      <c r="AQ1" s="73"/>
+      <c r="AR1" s="73"/>
+      <c r="AS1" s="73"/>
+      <c r="AT1" s="73"/>
+      <c r="AU1" s="73"/>
+      <c r="AV1" s="74"/>
       <c r="AW1" s="21"/>
-      <c r="AX1" s="49">
+      <c r="AX1" s="75">
         <v>2009</v>
       </c>
-      <c r="AY1" s="50"/>
-      <c r="AZ1" s="50"/>
-      <c r="BA1" s="50"/>
-      <c r="BB1" s="50"/>
-      <c r="BC1" s="50"/>
-      <c r="BD1" s="50"/>
-      <c r="BE1" s="51"/>
+      <c r="AY1" s="76"/>
+      <c r="AZ1" s="76"/>
+      <c r="BA1" s="76"/>
+      <c r="BB1" s="76"/>
+      <c r="BC1" s="76"/>
+      <c r="BD1" s="76"/>
+      <c r="BE1" s="77"/>
     </row>
     <row r="2" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="43" t="s">
+      <c r="C2" s="64"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="43" t="s">
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="55"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="43" t="s">
+      <c r="K2" s="60"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="44" t="s">
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="55"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="43" t="s">
+      <c r="S2" s="60"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="44"/>
-      <c r="W2" s="44"/>
-      <c r="X2" s="44"/>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="43" t="s">
+      <c r="V2" s="64"/>
+      <c r="W2" s="64"/>
+      <c r="X2" s="64"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="56"/>
-      <c r="AC2" s="43" t="s">
+      <c r="AA2" s="60"/>
+      <c r="AB2" s="45"/>
+      <c r="AC2" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
-      <c r="AF2" s="44"/>
-      <c r="AG2" s="45"/>
-      <c r="AH2" s="43" t="s">
+      <c r="AD2" s="64"/>
+      <c r="AE2" s="64"/>
+      <c r="AF2" s="64"/>
+      <c r="AG2" s="70"/>
+      <c r="AH2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="AI2" s="55"/>
-      <c r="AJ2" s="56"/>
-      <c r="AK2" s="43" t="s">
+      <c r="AI2" s="60"/>
+      <c r="AJ2" s="45"/>
+      <c r="AK2" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="45"/>
-      <c r="AP2" s="43" t="s">
+      <c r="AL2" s="64"/>
+      <c r="AM2" s="64"/>
+      <c r="AN2" s="64"/>
+      <c r="AO2" s="70"/>
+      <c r="AP2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="AQ2" s="55"/>
-      <c r="AR2" s="56"/>
-      <c r="AS2" s="43" t="s">
+      <c r="AQ2" s="60"/>
+      <c r="AR2" s="45"/>
+      <c r="AS2" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="AT2" s="44"/>
-      <c r="AU2" s="44"/>
-      <c r="AV2" s="44"/>
-      <c r="AW2" s="45"/>
-      <c r="AX2" s="43" t="s">
+      <c r="AT2" s="64"/>
+      <c r="AU2" s="64"/>
+      <c r="AV2" s="64"/>
+      <c r="AW2" s="70"/>
+      <c r="AX2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="AY2" s="55"/>
-      <c r="AZ2" s="56"/>
-      <c r="BA2" s="43" t="s">
+      <c r="AY2" s="60"/>
+      <c r="AZ2" s="45"/>
+      <c r="BA2" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="BB2" s="44"/>
-      <c r="BC2" s="44"/>
-      <c r="BD2" s="44"/>
-      <c r="BE2" s="45"/>
+      <c r="BB2" s="64"/>
+      <c r="BC2" s="64"/>
+      <c r="BD2" s="64"/>
+      <c r="BE2" s="70"/>
     </row>
     <row r="3" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A3" s="53"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58"/>
-      <c r="T3" s="59"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
-      <c r="Y3" s="48"/>
-      <c r="Z3" s="57"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="59"/>
-      <c r="AC3" s="46"/>
-      <c r="AD3" s="47"/>
-      <c r="AE3" s="47"/>
-      <c r="AF3" s="47"/>
-      <c r="AG3" s="48"/>
-      <c r="AH3" s="57"/>
-      <c r="AI3" s="58"/>
-      <c r="AJ3" s="59"/>
-      <c r="AK3" s="46"/>
-      <c r="AL3" s="47"/>
-      <c r="AM3" s="47"/>
-      <c r="AN3" s="47"/>
-      <c r="AO3" s="48"/>
-      <c r="AP3" s="57"/>
-      <c r="AQ3" s="58"/>
-      <c r="AR3" s="59"/>
-      <c r="AS3" s="46"/>
-      <c r="AT3" s="47"/>
-      <c r="AU3" s="47"/>
-      <c r="AV3" s="47"/>
-      <c r="AW3" s="48"/>
-      <c r="AX3" s="57"/>
-      <c r="AY3" s="58"/>
-      <c r="AZ3" s="59"/>
-      <c r="BA3" s="46"/>
-      <c r="BB3" s="47"/>
-      <c r="BC3" s="47"/>
-      <c r="BD3" s="47"/>
-      <c r="BE3" s="48"/>
+      <c r="A3" s="79"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="66"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="66"/>
+      <c r="W3" s="66"/>
+      <c r="X3" s="66"/>
+      <c r="Y3" s="71"/>
+      <c r="Z3" s="63"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="47"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="66"/>
+      <c r="AE3" s="66"/>
+      <c r="AF3" s="66"/>
+      <c r="AG3" s="71"/>
+      <c r="AH3" s="63"/>
+      <c r="AI3" s="59"/>
+      <c r="AJ3" s="47"/>
+      <c r="AK3" s="68"/>
+      <c r="AL3" s="66"/>
+      <c r="AM3" s="66"/>
+      <c r="AN3" s="66"/>
+      <c r="AO3" s="71"/>
+      <c r="AP3" s="63"/>
+      <c r="AQ3" s="59"/>
+      <c r="AR3" s="47"/>
+      <c r="AS3" s="68"/>
+      <c r="AT3" s="66"/>
+      <c r="AU3" s="66"/>
+      <c r="AV3" s="66"/>
+      <c r="AW3" s="71"/>
+      <c r="AX3" s="63"/>
+      <c r="AY3" s="59"/>
+      <c r="AZ3" s="47"/>
+      <c r="BA3" s="68"/>
+      <c r="BB3" s="66"/>
+      <c r="BC3" s="66"/>
+      <c r="BD3" s="66"/>
+      <c r="BE3" s="71"/>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="44" t="s">
+      <c r="A4" s="79"/>
+      <c r="B4" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="55" t="s">
+      <c r="F4" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="71"/>
-      <c r="H4" s="55" t="s">
+      <c r="G4" s="69"/>
+      <c r="H4" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="74"/>
-      <c r="J4" s="77" t="s">
+      <c r="I4" s="54"/>
+      <c r="J4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="80" t="s">
+      <c r="K4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="74" t="s">
+      <c r="L4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="64" t="s">
+      <c r="M4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="80" t="s">
+      <c r="N4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="80"/>
-      <c r="P4" s="80" t="s">
+      <c r="O4" s="51"/>
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="64" t="s">
+      <c r="Q4" s="45"/>
+      <c r="R4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="S4" s="80" t="s">
+      <c r="S4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="T4" s="74" t="s">
+      <c r="T4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="U4" s="64" t="s">
+      <c r="U4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="V4" s="80" t="s">
+      <c r="V4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="W4" s="55"/>
-      <c r="X4" s="80" t="s">
+      <c r="W4" s="60"/>
+      <c r="X4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Y4" s="56"/>
-      <c r="Z4" s="77" t="s">
+      <c r="Y4" s="45"/>
+      <c r="Z4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="AA4" s="80" t="s">
+      <c r="AA4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AB4" s="74" t="s">
+      <c r="AB4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="AC4" s="64" t="s">
+      <c r="AC4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="AD4" s="80" t="s">
+      <c r="AD4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AE4" s="55"/>
-      <c r="AF4" s="80" t="s">
+      <c r="AE4" s="60"/>
+      <c r="AF4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="AG4" s="56"/>
-      <c r="AH4" s="64" t="s">
+      <c r="AG4" s="45"/>
+      <c r="AH4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="AI4" s="80" t="s">
+      <c r="AI4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="74" t="s">
+      <c r="AJ4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="AK4" s="64" t="s">
+      <c r="AK4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="AL4" s="80" t="s">
+      <c r="AL4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AM4" s="55"/>
-      <c r="AN4" s="80" t="s">
+      <c r="AM4" s="60"/>
+      <c r="AN4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="AO4" s="56"/>
-      <c r="AP4" s="64" t="s">
+      <c r="AO4" s="45"/>
+      <c r="AP4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="AQ4" s="80" t="s">
+      <c r="AQ4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AR4" s="74" t="s">
+      <c r="AR4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="AS4" s="64" t="s">
+      <c r="AS4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="AT4" s="80" t="s">
+      <c r="AT4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AU4" s="55"/>
-      <c r="AV4" s="80" t="s">
+      <c r="AU4" s="60"/>
+      <c r="AV4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="AW4" s="56"/>
-      <c r="AX4" s="77" t="s">
+      <c r="AW4" s="45"/>
+      <c r="AX4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="AY4" s="80" t="s">
+      <c r="AY4" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AZ4" s="74" t="s">
+      <c r="AZ4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="BA4" s="81" t="s">
+      <c r="BA4" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="BB4" s="65" t="s">
+      <c r="BB4" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="BC4" s="68"/>
-      <c r="BD4" s="65" t="s">
+      <c r="BC4" s="58"/>
+      <c r="BD4" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="BE4" s="56"/>
+      <c r="BE4" s="45"/>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="65"/>
-      <c r="S5" s="72"/>
-      <c r="T5" s="75"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65"/>
-      <c r="W5" s="68"/>
-      <c r="X5" s="65"/>
-      <c r="Y5" s="69"/>
-      <c r="Z5" s="78"/>
-      <c r="AA5" s="72"/>
-      <c r="AB5" s="75"/>
-      <c r="AC5" s="65"/>
-      <c r="AD5" s="65"/>
-      <c r="AE5" s="68"/>
-      <c r="AF5" s="65"/>
-      <c r="AG5" s="69"/>
-      <c r="AH5" s="65"/>
-      <c r="AI5" s="72"/>
-      <c r="AJ5" s="75"/>
-      <c r="AK5" s="65"/>
-      <c r="AL5" s="72"/>
-      <c r="AM5" s="68"/>
-      <c r="AN5" s="65"/>
-      <c r="AO5" s="69"/>
-      <c r="AP5" s="65"/>
-      <c r="AQ5" s="72"/>
-      <c r="AR5" s="75"/>
-      <c r="AS5" s="65"/>
-      <c r="AT5" s="72"/>
-      <c r="AU5" s="68"/>
-      <c r="AV5" s="65"/>
-      <c r="AW5" s="69"/>
-      <c r="AX5" s="78"/>
-      <c r="AY5" s="72"/>
-      <c r="AZ5" s="75"/>
-      <c r="BA5" s="65"/>
-      <c r="BB5" s="72"/>
-      <c r="BC5" s="68"/>
-      <c r="BD5" s="65"/>
-      <c r="BE5" s="69"/>
+      <c r="A5" s="79"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="52"/>
+      <c r="T5" s="55"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="58"/>
+      <c r="X5" s="43"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="49"/>
+      <c r="AA5" s="52"/>
+      <c r="AB5" s="55"/>
+      <c r="AC5" s="43"/>
+      <c r="AD5" s="43"/>
+      <c r="AE5" s="58"/>
+      <c r="AF5" s="43"/>
+      <c r="AG5" s="46"/>
+      <c r="AH5" s="43"/>
+      <c r="AI5" s="52"/>
+      <c r="AJ5" s="55"/>
+      <c r="AK5" s="43"/>
+      <c r="AL5" s="52"/>
+      <c r="AM5" s="58"/>
+      <c r="AN5" s="43"/>
+      <c r="AO5" s="46"/>
+      <c r="AP5" s="43"/>
+      <c r="AQ5" s="52"/>
+      <c r="AR5" s="55"/>
+      <c r="AS5" s="43"/>
+      <c r="AT5" s="52"/>
+      <c r="AU5" s="58"/>
+      <c r="AV5" s="43"/>
+      <c r="AW5" s="46"/>
+      <c r="AX5" s="49"/>
+      <c r="AY5" s="52"/>
+      <c r="AZ5" s="55"/>
+      <c r="BA5" s="43"/>
+      <c r="BB5" s="52"/>
+      <c r="BC5" s="58"/>
+      <c r="BD5" s="43"/>
+      <c r="BE5" s="46"/>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="65"/>
-      <c r="S6" s="72"/>
-      <c r="T6" s="75"/>
-      <c r="U6" s="65"/>
-      <c r="V6" s="65"/>
-      <c r="W6" s="68"/>
-      <c r="X6" s="65"/>
-      <c r="Y6" s="69"/>
-      <c r="Z6" s="78"/>
-      <c r="AA6" s="72"/>
-      <c r="AB6" s="75"/>
-      <c r="AC6" s="65"/>
-      <c r="AD6" s="65"/>
-      <c r="AE6" s="68"/>
-      <c r="AF6" s="65"/>
-      <c r="AG6" s="69"/>
-      <c r="AH6" s="65"/>
-      <c r="AI6" s="72"/>
-      <c r="AJ6" s="75"/>
-      <c r="AK6" s="65"/>
-      <c r="AL6" s="72"/>
-      <c r="AM6" s="68"/>
-      <c r="AN6" s="65"/>
-      <c r="AO6" s="69"/>
-      <c r="AP6" s="65"/>
-      <c r="AQ6" s="72"/>
-      <c r="AR6" s="75"/>
-      <c r="AS6" s="65"/>
-      <c r="AT6" s="72"/>
-      <c r="AU6" s="68"/>
-      <c r="AV6" s="65"/>
-      <c r="AW6" s="69"/>
-      <c r="AX6" s="78"/>
-      <c r="AY6" s="72"/>
-      <c r="AZ6" s="75"/>
-      <c r="BA6" s="65"/>
-      <c r="BB6" s="72"/>
-      <c r="BC6" s="68"/>
-      <c r="BD6" s="65"/>
-      <c r="BE6" s="69"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="52"/>
+      <c r="T6" s="55"/>
+      <c r="U6" s="43"/>
+      <c r="V6" s="43"/>
+      <c r="W6" s="58"/>
+      <c r="X6" s="43"/>
+      <c r="Y6" s="46"/>
+      <c r="Z6" s="49"/>
+      <c r="AA6" s="52"/>
+      <c r="AB6" s="55"/>
+      <c r="AC6" s="43"/>
+      <c r="AD6" s="43"/>
+      <c r="AE6" s="58"/>
+      <c r="AF6" s="43"/>
+      <c r="AG6" s="46"/>
+      <c r="AH6" s="43"/>
+      <c r="AI6" s="52"/>
+      <c r="AJ6" s="55"/>
+      <c r="AK6" s="43"/>
+      <c r="AL6" s="52"/>
+      <c r="AM6" s="58"/>
+      <c r="AN6" s="43"/>
+      <c r="AO6" s="46"/>
+      <c r="AP6" s="43"/>
+      <c r="AQ6" s="52"/>
+      <c r="AR6" s="55"/>
+      <c r="AS6" s="43"/>
+      <c r="AT6" s="52"/>
+      <c r="AU6" s="58"/>
+      <c r="AV6" s="43"/>
+      <c r="AW6" s="46"/>
+      <c r="AX6" s="49"/>
+      <c r="AY6" s="52"/>
+      <c r="AZ6" s="55"/>
+      <c r="BA6" s="43"/>
+      <c r="BB6" s="52"/>
+      <c r="BC6" s="58"/>
+      <c r="BD6" s="43"/>
+      <c r="BE6" s="46"/>
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="76"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
-      <c r="O7" s="66"/>
-      <c r="P7" s="66"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="66"/>
-      <c r="S7" s="73"/>
-      <c r="T7" s="76"/>
-      <c r="U7" s="66"/>
-      <c r="V7" s="66"/>
-      <c r="W7" s="58"/>
-      <c r="X7" s="66"/>
-      <c r="Y7" s="59"/>
-      <c r="Z7" s="79"/>
-      <c r="AA7" s="73"/>
-      <c r="AB7" s="76"/>
-      <c r="AC7" s="66"/>
-      <c r="AD7" s="66"/>
-      <c r="AE7" s="58"/>
-      <c r="AF7" s="66"/>
-      <c r="AG7" s="59"/>
-      <c r="AH7" s="66"/>
-      <c r="AI7" s="73"/>
-      <c r="AJ7" s="76"/>
-      <c r="AK7" s="66"/>
-      <c r="AL7" s="73"/>
-      <c r="AM7" s="58"/>
-      <c r="AN7" s="66"/>
-      <c r="AO7" s="59"/>
-      <c r="AP7" s="66"/>
-      <c r="AQ7" s="73"/>
-      <c r="AR7" s="76"/>
-      <c r="AS7" s="66"/>
-      <c r="AT7" s="73"/>
-      <c r="AU7" s="58"/>
-      <c r="AV7" s="66"/>
-      <c r="AW7" s="59"/>
-      <c r="AX7" s="79"/>
-      <c r="AY7" s="73"/>
-      <c r="AZ7" s="76"/>
-      <c r="BA7" s="66"/>
-      <c r="BB7" s="73"/>
-      <c r="BC7" s="58"/>
-      <c r="BD7" s="66"/>
-      <c r="BE7" s="59"/>
+      <c r="A7" s="80"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="44"/>
+      <c r="S7" s="53"/>
+      <c r="T7" s="56"/>
+      <c r="U7" s="44"/>
+      <c r="V7" s="44"/>
+      <c r="W7" s="59"/>
+      <c r="X7" s="44"/>
+      <c r="Y7" s="47"/>
+      <c r="Z7" s="50"/>
+      <c r="AA7" s="53"/>
+      <c r="AB7" s="56"/>
+      <c r="AC7" s="44"/>
+      <c r="AD7" s="44"/>
+      <c r="AE7" s="59"/>
+      <c r="AF7" s="44"/>
+      <c r="AG7" s="47"/>
+      <c r="AH7" s="44"/>
+      <c r="AI7" s="53"/>
+      <c r="AJ7" s="56"/>
+      <c r="AK7" s="44"/>
+      <c r="AL7" s="53"/>
+      <c r="AM7" s="59"/>
+      <c r="AN7" s="44"/>
+      <c r="AO7" s="47"/>
+      <c r="AP7" s="44"/>
+      <c r="AQ7" s="53"/>
+      <c r="AR7" s="56"/>
+      <c r="AS7" s="44"/>
+      <c r="AT7" s="53"/>
+      <c r="AU7" s="59"/>
+      <c r="AV7" s="44"/>
+      <c r="AW7" s="47"/>
+      <c r="AX7" s="50"/>
+      <c r="AY7" s="53"/>
+      <c r="AZ7" s="56"/>
+      <c r="BA7" s="44"/>
+      <c r="BB7" s="53"/>
+      <c r="BC7" s="59"/>
+      <c r="BD7" s="44"/>
+      <c r="BE7" s="47"/>
     </row>
     <row r="8" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
@@ -5821,26 +5824,48 @@
     <sortCondition descending="1" ref="K23"/>
   </sortState>
   <mergeCells count="78">
-    <mergeCell ref="BD4:BD7"/>
-    <mergeCell ref="BE4:BE7"/>
-    <mergeCell ref="AX4:AX7"/>
-    <mergeCell ref="AY4:AY7"/>
-    <mergeCell ref="AZ4:AZ7"/>
-    <mergeCell ref="BA4:BA7"/>
-    <mergeCell ref="BB4:BB7"/>
-    <mergeCell ref="BC4:BC7"/>
-    <mergeCell ref="AW4:AW7"/>
-    <mergeCell ref="AL4:AL7"/>
-    <mergeCell ref="AM4:AM7"/>
-    <mergeCell ref="AN4:AN7"/>
-    <mergeCell ref="AO4:AO7"/>
-    <mergeCell ref="AP4:AP7"/>
-    <mergeCell ref="AQ4:AQ7"/>
-    <mergeCell ref="AR4:AR7"/>
-    <mergeCell ref="AS4:AS7"/>
-    <mergeCell ref="AT4:AT7"/>
-    <mergeCell ref="AU4:AU7"/>
-    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="BA2:BE3"/>
+    <mergeCell ref="AX1:BE1"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E2:I3"/>
+    <mergeCell ref="J2:L3"/>
+    <mergeCell ref="M2:Q3"/>
+    <mergeCell ref="R2:T3"/>
+    <mergeCell ref="U2:Y3"/>
+    <mergeCell ref="Z2:AB3"/>
+    <mergeCell ref="AC2:AG3"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="R1:Y1"/>
+    <mergeCell ref="Z1:AG1"/>
+    <mergeCell ref="AH1:AN1"/>
+    <mergeCell ref="AH2:AJ3"/>
+    <mergeCell ref="AK2:AO3"/>
+    <mergeCell ref="AP2:AR3"/>
+    <mergeCell ref="AS2:AW3"/>
+    <mergeCell ref="AP1:AV1"/>
+    <mergeCell ref="AX2:AZ3"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="Y4:Y7"/>
+    <mergeCell ref="N4:N7"/>
+    <mergeCell ref="O4:O7"/>
+    <mergeCell ref="P4:P7"/>
+    <mergeCell ref="Q4:Q7"/>
+    <mergeCell ref="R4:R7"/>
+    <mergeCell ref="S4:S7"/>
+    <mergeCell ref="T4:T7"/>
     <mergeCell ref="U4:U7"/>
     <mergeCell ref="V4:V7"/>
     <mergeCell ref="W4:W7"/>
@@ -5857,48 +5882,26 @@
     <mergeCell ref="AH4:AH7"/>
     <mergeCell ref="AI4:AI7"/>
     <mergeCell ref="AJ4:AJ7"/>
-    <mergeCell ref="P4:P7"/>
-    <mergeCell ref="Q4:Q7"/>
-    <mergeCell ref="R4:R7"/>
-    <mergeCell ref="S4:S7"/>
-    <mergeCell ref="T4:T7"/>
-    <mergeCell ref="AX2:AZ3"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="Y4:Y7"/>
-    <mergeCell ref="N4:N7"/>
-    <mergeCell ref="O4:O7"/>
-    <mergeCell ref="AH2:AJ3"/>
-    <mergeCell ref="AK2:AO3"/>
-    <mergeCell ref="AP2:AR3"/>
-    <mergeCell ref="AS2:AW3"/>
-    <mergeCell ref="AP1:AV1"/>
-    <mergeCell ref="BA2:BE3"/>
-    <mergeCell ref="AX1:BE1"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:D3"/>
-    <mergeCell ref="E2:I3"/>
-    <mergeCell ref="J2:L3"/>
-    <mergeCell ref="M2:Q3"/>
-    <mergeCell ref="R2:T3"/>
-    <mergeCell ref="U2:Y3"/>
-    <mergeCell ref="Z2:AB3"/>
-    <mergeCell ref="AC2:AG3"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:Y1"/>
-    <mergeCell ref="Z1:AG1"/>
-    <mergeCell ref="AH1:AN1"/>
+    <mergeCell ref="AW4:AW7"/>
+    <mergeCell ref="AL4:AL7"/>
+    <mergeCell ref="AM4:AM7"/>
+    <mergeCell ref="AN4:AN7"/>
+    <mergeCell ref="AO4:AO7"/>
+    <mergeCell ref="AP4:AP7"/>
+    <mergeCell ref="AQ4:AQ7"/>
+    <mergeCell ref="AR4:AR7"/>
+    <mergeCell ref="AS4:AS7"/>
+    <mergeCell ref="AT4:AT7"/>
+    <mergeCell ref="AU4:AU7"/>
+    <mergeCell ref="AV4:AV7"/>
+    <mergeCell ref="BD4:BD7"/>
+    <mergeCell ref="BE4:BE7"/>
+    <mergeCell ref="AX4:AX7"/>
+    <mergeCell ref="AY4:AY7"/>
+    <mergeCell ref="AZ4:AZ7"/>
+    <mergeCell ref="BA4:BA7"/>
+    <mergeCell ref="BB4:BB7"/>
+    <mergeCell ref="BC4:BC7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>